<commit_message>
Added ADV_11, removed ADV_12
Added ADV_11, removed ADV_12
</commit_message>
<xml_diff>
--- a/10_MultipleActions/Default.xlsx
+++ b/10_MultipleActions/Default.xlsx
@@ -205,9 +205,7 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -216,7 +214,9 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -252,13 +252,13 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyProtection="1">
@@ -560,18 +560,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="8.8984375" style="1" customWidth="1"/>
+    <col min="1" max="3" width="9.41796875" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.8984375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.95" customFormat="1"/>
+    <row r="1" ht="14.95" s="4" customFormat="1">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -582,26 +593,26 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="11.4375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.91796875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.31640625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.8984375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.4375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.91796875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20.31640625" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="8.8984375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.95" s="4" customFormat="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="5" t="s">
@@ -609,13 +620,13 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="6" t="s">
@@ -623,37 +634,37 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="6"/>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="6"/>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="6"/>
@@ -673,7 +684,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.95"/>
   <cols>
-    <col min="1" max="16384" width="8.8984375" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="8.8984375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1"/>
@@ -692,7 +703,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.95" customFormat="1"/>

</xml_diff>